<commit_message>
Adding a bunch of art
</commit_message>
<xml_diff>
--- a/data/Orcus - Arts.xlsx
+++ b/data/Orcus - Arts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Obsidian\Tabletop games\d20 System or D&amp;D-esque\2021 Orcus - 4E clone\GitHub\orcus\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774CEB54-72F8-4862-8368-82A8C24845C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706E93B3-5F76-4BD8-976A-ECD77B54C27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -573,9 +572,6 @@
     <t xml:space="preserve">The target of the incantation is brought back to life, with the Revenant bond. Make a Religion check. The result determines what starting Favor the target begins with. *Religion result 10 or less:* -3 Favor. *Religion result 11-15:* 0 Favor. *Religion result 16-20:* 5 Favor. *Religion result 21-25:* 10 Favor. *Religion result 26 or more:* 15 Favor. </t>
   </si>
   <si>
-    <t xml:space="preserve">The target of the experimental resurrection is brought back to life. The subject must have died within the last 24 hours, and their body must be intact. </t>
-  </si>
-  <si>
     <t>14 gp</t>
   </si>
   <si>
@@ -773,12 +769,6 @@
   <si>
     <t>This incantation grants a willing creature the ability to breathe underwater until the incantation ends. Affected creatures also retain their normal mode of respiration.   
 **Arcana check:** With a DC 15 Arcana check, you can choose up to 10 targets for this incantation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Hrothgar’s journey* is an incantation based on the tale of Hrothgar, a powerful barbarian hero from ages past. When the poetic epic of Hrothgar is recited in the stifling heat of a sweat lodge during the winter solstice, the orator and his listeners receive the same final reward that Hrothgar did: a one-way trip to Asgard’s Valhalla, where they can drink and make merry with the greatest warriors of myth.  
-To cast the incantation, the caster must construct a small, windowless hut in the middle of the forest, then build a bonfire in the hut’s center. At least four and up to twelve others accompany the caster into the hut. Other participants must provide the dialogue for other characters in the epic of Hrothgar. Then the flames are lit and the telling of the tale of Hrothgar begins.  
-Because the bonfire is large and the hut is small, the atmosphere inside quickly gets stiflingly hot. Any creature inside the hut must make an Endure check (DC 20) every 10 minutes or suffer the effects of severe heat (lose a recovery).  
-Just as the tale of Hrothgar approaches its conclusion (near the end of the casting time), the bonfire’s flames light the hut on fire, which creates a great deal of smoke but no additional heat or damage. The flames consume the hut’s roof and walls, revealing Valhalla. If the caster succeeds on a DC 19 Arcana check, they can choose the exact location in Valhalla that the party appears.  </t>
   </si>
   <si>
     <t xml:space="preserve">You and up to eight willing creatures who link hands in a circle are transported to a different plane of existence. You can specify a target destination in general terms, such as the City of Brass on the Elemental Plane of Fire, and you appear in or near that destination.   
@@ -1019,6 +1009,17 @@
   </si>
   <si>
     <t>You establish a safe house—a secure space in which to hide your secrets from the outside world. This safe house is roughly the size of a 10-foot cube. It’s in a location you have access to, and it can be part of a larger building or structure, like a hidden room or an underground cave. The safe house protects objects and people inside it from magical detection. Setting up or moving your safe house takes a week of downtime. The size of the safe house expands by one 10-foot cube each time you use this craft.</t>
+  </si>
+  <si>
+    <t>*Hrothgar’s journey* is an incantation based on the tale of Hrothgar, a powerful barbarian hero from ages past. When the poetic epic of Hrothgar is recited in the stifling heat of a sweat lodge during the winter solstice, the orator and his listeners receive the same final reward that Hrothgar did: a one-way trip to Asgard’s Valhalla, where they can drink and make merry with the greatest warriors of myth.  
+To cast the incantation, the caster must construct a small, windowless hut in the middle of the forest, then build a bonfire in the hut’s center. At least four and up to twelve others accompany the caster into the hut. Other participants must provide the dialogue for other characters in the epic of Hrothgar. Then the flames are lit and the telling of the tale of Hrothgar begins.  
+Because the bonfire is large and the hut is small, the atmosphere inside quickly gets stiflingly hot. Any creature inside the hut must make an Endure check (DC 20) every 10 minutes or suffer the effects of severe heat (lose a recovery).  
+Just as the tale of Hrothgar approaches its conclusion (near the end of the casting time), the bonfire’s flames light the hut on fire, which creates a great deal of smoke but no additional heat or damage. The flames consume the hut’s roof and walls, revealing Valhalla. If the caster succeeds on a DC 19 Arcana check, they can choose the exact location in Valhalla that the party appears.  
+&lt;figure&gt;&lt;img src="pics\LuigiCastellani_LOKOSSAPALACE.png" alt="Palace by Luigi Castellani" style="zoom: 100%;" /&gt;&lt;figcaption&gt;Palace by Luigi Castellani&lt;/figcaption&gt;&lt;/figure&gt;</t>
+  </si>
+  <si>
+    <t>The target of the experimental resurrection is brought back to life. The subject must have died within the last 24 hours, and their body must be intact. 
+&lt;figure&gt;&lt;img src="pics\JoyceMaureira_MAGSPELL1.png" alt="Magic Spell 1 by Joyce Maureira" style="zoom: 33%;" /&gt;&lt;figcaption&gt;Magic Spell 1 by Joyce Maureira&lt;/figcaption&gt;&lt;/figure&gt;</t>
   </si>
 </sst>
 </file>
@@ -1345,10 +1346,10 @@
   <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1425,13 +1426,13 @@
         <v>123</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>78</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1457,13 +1458,13 @@
         <v>126</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1489,13 +1490,13 @@
         <v>145</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1521,18 +1522,18 @@
         <v>127</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -1550,16 +1551,16 @@
         <v>31</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>102</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1585,13 +1586,13 @@
         <v>128</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1617,13 +1618,13 @@
         <v>129</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>78</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1649,13 +1650,13 @@
         <v>147</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>102</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1678,16 +1679,16 @@
         <v>12</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>78</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1713,7 +1714,7 @@
         <v>148</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>14</v>
@@ -1724,7 +1725,7 @@
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B13" s="1">
         <v>5</v>
@@ -1742,16 +1743,16 @@
         <v>31</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1777,13 +1778,13 @@
         <v>137</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>78</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1806,16 +1807,16 @@
         <v>12</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>78</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1841,13 +1842,13 @@
         <v>136</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1870,16 +1871,16 @@
         <v>12</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>78</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1905,13 +1906,13 @@
         <v>134</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>78</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1934,16 +1935,16 @@
         <v>12</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>31</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1966,21 +1967,21 @@
         <v>12</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>78</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B21" s="1">
         <v>11</v>
@@ -2001,13 +2002,13 @@
         <v>140</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>235</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2033,13 +2034,13 @@
         <v>151</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>102</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2065,13 +2066,13 @@
         <v>139</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>78</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2097,13 +2098,13 @@
         <v>138</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2126,16 +2127,16 @@
         <v>15</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>102</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2172,7 +2173,7 @@
         <v>32</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>41</v>
@@ -2194,7 +2195,7 @@
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
@@ -2212,16 +2213,16 @@
         <v>19</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2244,10 +2245,10 @@
         <v>45</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>171</v>
@@ -2279,13 +2280,13 @@
         <v>32</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2308,16 +2309,16 @@
         <v>45</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I32" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2343,13 +2344,13 @@
         <v>149</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2372,16 +2373,16 @@
         <v>19</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2397,7 +2398,7 @@
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
@@ -2415,16 +2416,16 @@
         <v>19</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2450,7 +2451,7 @@
         <v>32</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>14</v>
@@ -2479,10 +2480,10 @@
         <v>19</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>14</v>
@@ -2525,7 +2526,7 @@
         <v>32</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>14</v>
@@ -2557,7 +2558,7 @@
         <v>32</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>14</v>
@@ -2589,7 +2590,7 @@
         <v>32</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>14</v>
@@ -2621,7 +2622,7 @@
         <v>32</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>14</v>
@@ -2653,7 +2654,7 @@
         <v>32</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>14</v>
@@ -2697,13 +2698,13 @@
         <v>124</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>33</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2726,16 +2727,16 @@
         <v>12</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2761,13 +2762,13 @@
         <v>150</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2793,13 +2794,13 @@
         <v>152</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J49" s="1" t="s">
-        <v>178</v>
+      <c r="J49" s="4" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2810,12 +2811,12 @@
         <v>0</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B51" s="1">
         <v>3</v>
@@ -2827,22 +2828,22 @@
         <v>155</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2879,13 +2880,13 @@
         <v>32</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2922,13 +2923,13 @@
         <v>125</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>45</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2954,13 +2955,13 @@
         <v>32</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2983,16 +2984,16 @@
         <v>12</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3015,16 +3016,16 @@
         <v>12</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3050,13 +3051,13 @@
         <v>21</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3082,13 +3083,13 @@
         <v>130</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>31</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3114,13 +3115,13 @@
         <v>131</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>79</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3146,13 +3147,13 @@
         <v>133</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3178,13 +3179,13 @@
         <v>83</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3207,16 +3208,16 @@
         <v>12</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>78</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3242,13 +3243,13 @@
         <v>32</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>41</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3271,16 +3272,16 @@
         <v>12</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3323,12 +3324,12 @@
         <v>14</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B69" s="1">
         <v>1</v>
@@ -3355,7 +3356,7 @@
         <v>14</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3381,7 +3382,7 @@
         <v>32</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>69</v>
@@ -3419,7 +3420,7 @@
         <v>14</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3451,7 +3452,7 @@
         <v>14</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3477,7 +3478,7 @@
         <v>21</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>102</v>
@@ -3499,7 +3500,7 @@
     </row>
     <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B75" s="1">
         <v>1</v>
@@ -3517,21 +3518,21 @@
         <v>45</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>45</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B76" s="1">
         <v>1</v>
@@ -3552,13 +3553,13 @@
         <v>32</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3584,13 +3585,13 @@
         <v>132</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3613,16 +3614,16 @@
         <v>12</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3648,13 +3649,13 @@
         <v>135</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>45</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3680,18 +3681,18 @@
         <v>144</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B81" s="1">
         <v>9</v>
@@ -3712,13 +3713,13 @@
         <v>143</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3744,13 +3745,13 @@
         <v>141</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>69</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3776,13 +3777,13 @@
         <v>38</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>39</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3808,7 +3809,7 @@
         <v>176</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>14</v>
@@ -3819,7 +3820,7 @@
     </row>
     <row r="85" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B85" s="1">
         <v>21</v>
@@ -3840,13 +3841,13 @@
         <v>142</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>78</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3889,7 +3890,7 @@
         <v>14</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3923,10 +3924,10 @@
         <v>45</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>45</v>
@@ -3948,7 +3949,7 @@
     </row>
     <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B91" s="1">
         <v>1</v>
@@ -3963,19 +3964,19 @@
         <v>50</v>
       </c>
       <c r="F91" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G91" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="G91" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="H91" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3998,16 +3999,16 @@
         <v>12</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4033,7 +4034,7 @@
         <v>146</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>14</v>
@@ -4062,16 +4063,16 @@
         <v>51</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4094,16 +4095,16 @@
         <v>19</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -4175,7 +4176,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -4217,7 +4218,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -4343,7 +4344,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -4385,7 +4386,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
@@ -4399,7 +4400,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -4455,7 +4456,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
@@ -4637,7 +4638,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B37" s="1">
         <v>3</v>
@@ -4646,7 +4647,7 @@
         <v>155</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -4763,7 +4764,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B46" s="1">
         <v>5</v>
@@ -5043,7 +5044,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B66" s="1">
         <v>9</v>
@@ -5253,7 +5254,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B81" s="1">
         <v>21</v>

</xml_diff>

<commit_message>
Fixing tag language, adding descriptions to most monsters, etc
</commit_message>
<xml_diff>
--- a/data/Orcus - Arts.xlsx
+++ b/data/Orcus - Arts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Obsidian\Tabletop games\d20 System or D&amp;D-esque\2021 Orcus - 4E clone\GitHub\orcus\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92DBD9E-A260-4C86-842E-CE42F25C7F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B4D735-19C8-44C1-95E3-E4592765F2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -632,10 +632,6 @@
     <t>Detect Otherworldly</t>
   </si>
   <si>
-    <t>For the duration, you know if there is a creature of the cosmic, elemental, fey, outsider or shadow source or with the celestial, demon, devil or undead tags within 6 squares of you, as well as where the creature is located. Similarly, you know if there is a place or object within 6 squares of you that has been magically consecrated or desecrated.
-The incantation can penetrate most barriers, but it is blocked by 1 foot of stone, 1 inch of common metal, a thin sheet of lead, or 3 feet of wood or dirt.</t>
-  </si>
-  <si>
     <t>History</t>
   </si>
   <si>
@@ -700,12 +696,6 @@
 - *Nothing*, for results that aren’t especially good or bad  
 The incantation doesn’t take into account any possible circumstances that might change the outcome.  
 If you cast the incantation two or more times before completing your next long rest, there is a cumulative 25 percent chance for each casting after the first that you get a random reading. The GM makes this roll in secret.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">You create a ward against magical travel that protects up to 1,600 squares of floor space to a height of 6 squares above the floor. For the duration, creatures can’t teleport into the area or use portals to enter the area. The incantation proofs the area against planar travel, and therefore prevents creatures from accessing the area by way of the Astral Plane, Ethereal Plane, Plane of Faerie, Plane of Shadow, or the *plane walk* incantation.  
-In addition, the incantation damages types of creatures that you choose when you cast it. Choose one or more of the following tags: air, celestial, cold, demon, devil, earth, fire, water or undead. When a creature with that tag enters the incantation’s area for the first time on a turn or starts its turn there, the creature takes 5d10 radiant or necrotic damage (your choice when you cast this incantation).  
-When you cast this incantation, you can designate a password. A creature that speaks the password as it enters the area takes no damage from the incantation.  
-The incantation’s area can’t overlap with the area of another *forbid intrusion* incantation. If you cast *forbid intrusion* every day for 7 days in the same location, the incantation lasts until it is dispelled.  </t>
   </si>
   <si>
     <t>This incantation, dreamed up by cultists, opens a fell rift between the current location and a fiery layer of the Abyss. This rift brings about a massive conflagration that destroys almost everything in the immediate area, then releases a powerful demon who capers over the smoldering ruins and begins to rampage across the countryside. The *fires of the Abyss* ignite everything they touch—except for the caster, who is knocked unconscious and transported to a layer of the Abyss.  
@@ -1072,6 +1062,16 @@
 If the instructions involve some open-ended task that the recipient cannot complete through their own actions the craft remains in effect for a maximum of one day per level you have. A clever recipient can subvert some instructions.
 If the subject is prevented from obeying the *geas* for 24 hours, it loses one recovery. It cannot regain this recovery while the geas remains.
 *Religion check:* With a moderate DC Religion check (based on the level of the target), you can target a creature of level higher than your own. </t>
+  </si>
+  <si>
+    <t>For the duration, you know if there is a creature of the cosmic, elemental, fey, outsider or shadow source or with the Celestial, Demon, Devil or Undead tags within 6 squares of you, as well as where the creature is located. Similarly, you know if there is a place or object within 6 squares of you that has been magically consecrated or desecrated.
+The incantation can penetrate most barriers, but it is blocked by 1 foot of stone, 1 inch of common metal, a thin sheet of lead, or 3 feet of wood or dirt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You create a ward against magical travel that protects up to 1,600 squares of floor space to a height of 6 squares above the floor. For the duration, creatures can’t teleport into the area or use portals to enter the area. The incantation proofs the area against planar travel, and therefore prevents creatures from accessing the area by way of the Astral Plane, Ethereal Plane, Plane of Faerie, Plane of Shadow, or the *plane walk* incantation.  
+In addition, the incantation damages types of creatures that you choose when you cast it. Choose one or more of the following tags: Air, Celestial, Cold, Demon, Devil, Earth, Fire, Water or Undead. When a creature with that tag enters the incantation’s area for the first time on a turn or starts its turn there, the creature takes 5d10 radiant or necrotic damage (your choice when you cast this incantation).  
+When you cast this incantation, you can designate a password. A creature that speaks the password as it enters the area takes no damage from the incantation.  
+The incantation’s area can’t overlap with the area of another *forbid intrusion* incantation. If you cast *forbid intrusion* every day for 7 days in the same location, the incantation lasts until it is dispelled.  </t>
   </si>
 </sst>
 </file>
@@ -1403,10 +1403,10 @@
   <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B80" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J98" sqref="J98"/>
+      <selection pane="bottomRight" activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1487,7 +1487,7 @@
         <v>76</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1519,7 +1519,7 @@
         <v>76</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1551,7 +1551,7 @@
         <v>14</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1583,12 +1583,12 @@
         <v>32</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1615,7 +1615,7 @@
         <v>99</v>
       </c>
       <c r="J7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1647,7 +1647,7 @@
         <v>12</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1679,7 +1679,7 @@
         <v>76</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1711,7 +1711,7 @@
         <v>99</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1734,7 +1734,7 @@
         <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H11" t="s">
         <v>169</v>
@@ -1743,7 +1743,7 @@
         <v>76</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1798,7 +1798,7 @@
         <v>30</v>
       </c>
       <c r="G13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H13" t="s">
         <v>171</v>
@@ -1807,7 +1807,7 @@
         <v>14</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1830,7 +1830,7 @@
         <v>44</v>
       </c>
       <c r="G14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H14" t="s">
         <v>170</v>
@@ -1839,7 +1839,7 @@
         <v>76</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1862,7 +1862,7 @@
         <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H15" t="s">
         <v>170</v>
@@ -1871,7 +1871,7 @@
         <v>76</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1903,7 +1903,7 @@
         <v>15</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1926,7 +1926,7 @@
         <v>44</v>
       </c>
       <c r="G17" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H17" t="s">
         <v>170</v>
@@ -1935,7 +1935,7 @@
         <v>76</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1967,7 +1967,7 @@
         <v>76</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1990,16 +1990,16 @@
         <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H19" t="s">
         <v>172</v>
       </c>
       <c r="I19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2028,7 +2028,7 @@
         <v>173</v>
       </c>
       <c r="I20" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>185</v>
@@ -2036,7 +2036,7 @@
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B21">
         <v>11</v>
@@ -2063,7 +2063,7 @@
         <v>14</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2095,7 +2095,7 @@
         <v>99</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2127,7 +2127,7 @@
         <v>76</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2159,7 +2159,7 @@
         <v>14</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2182,7 +2182,7 @@
         <v>15</v>
       </c>
       <c r="G25" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H25" t="s">
         <v>188</v>
@@ -2191,7 +2191,7 @@
         <v>99</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2329,7 +2329,7 @@
         <v>17</v>
       </c>
       <c r="F31" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G31" t="s">
         <v>31</v>
@@ -2341,7 +2341,7 @@
         <v>14</v>
       </c>
       <c r="J31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2364,7 +2364,7 @@
         <v>44</v>
       </c>
       <c r="G32" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H32" t="s">
         <v>171</v>
@@ -2396,7 +2396,7 @@
         <v>19</v>
       </c>
       <c r="G33" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H33" t="s">
         <v>171</v>
@@ -2405,7 +2405,7 @@
         <v>14</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2428,7 +2428,7 @@
         <v>19</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>189</v>
@@ -2437,7 +2437,7 @@
         <v>14</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2535,7 +2535,7 @@
         <v>19</v>
       </c>
       <c r="G38" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H38" t="s">
         <v>176</v>
@@ -2683,7 +2683,7 @@
         <v>14</v>
       </c>
       <c r="J43" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2750,7 +2750,7 @@
         <v>12</v>
       </c>
       <c r="G46" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H46" t="s">
         <v>168</v>
@@ -2759,7 +2759,7 @@
         <v>32</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2782,7 +2782,7 @@
         <v>12</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>168</v>
@@ -2791,7 +2791,7 @@
         <v>14</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2823,7 +2823,7 @@
         <v>14</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2855,7 +2855,7 @@
         <v>14</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2866,12 +2866,12 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -2883,13 +2883,13 @@
         <v>146</v>
       </c>
       <c r="E51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F51" t="s">
         <v>44</v>
       </c>
       <c r="G51" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H51" t="s">
         <v>169</v>
@@ -2898,7 +2898,7 @@
         <v>14</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2941,7 +2941,7 @@
         <v>14</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3016,7 +3016,7 @@
         <v>14</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3039,7 +3039,7 @@
         <v>12</v>
       </c>
       <c r="G57" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H57" t="s">
         <v>168</v>
@@ -3071,7 +3071,7 @@
         <v>12</v>
       </c>
       <c r="G58" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H58" t="s">
         <v>168</v>
@@ -3080,7 +3080,7 @@
         <v>12</v>
       </c>
       <c r="J58" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3103,7 +3103,7 @@
         <v>19</v>
       </c>
       <c r="G59" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H59" t="s">
         <v>168</v>
@@ -3112,7 +3112,7 @@
         <v>14</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3144,7 +3144,7 @@
         <v>30</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3176,7 +3176,7 @@
         <v>77</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3208,7 +3208,7 @@
         <v>14</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3231,7 +3231,7 @@
         <v>76</v>
       </c>
       <c r="G63" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H63" t="s">
         <v>170</v>
@@ -3240,7 +3240,7 @@
         <v>14</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3263,7 +3263,7 @@
         <v>44</v>
       </c>
       <c r="G64" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H64" t="s">
         <v>170</v>
@@ -3272,7 +3272,7 @@
         <v>76</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3304,7 +3304,7 @@
         <v>40</v>
       </c>
       <c r="J65" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3327,7 +3327,7 @@
         <v>12</v>
       </c>
       <c r="G66" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H66" t="s">
         <v>172</v>
@@ -3336,7 +3336,7 @@
         <v>14</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3370,16 +3370,16 @@
         <v>12</v>
       </c>
       <c r="G68" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H68" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I68" t="s">
         <v>14</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3402,16 +3402,16 @@
         <v>12</v>
       </c>
       <c r="G69" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H69" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I69" t="s">
         <v>14</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3448,7 +3448,7 @@
     </row>
     <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B71">
         <v>2</v>
@@ -3466,16 +3466,16 @@
         <v>19</v>
       </c>
       <c r="G71" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H71" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I71" t="s">
         <v>14</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3498,16 +3498,16 @@
         <v>19</v>
       </c>
       <c r="G72" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H72" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I72" t="s">
         <v>14</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3530,13 +3530,13 @@
         <v>76</v>
       </c>
       <c r="G73" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H73" t="s">
         <v>170</v>
       </c>
       <c r="I73" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J73" t="s">
         <v>151</v>
@@ -3573,7 +3573,7 @@
         <v>44</v>
       </c>
       <c r="G75" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H75" t="s">
         <v>168</v>
@@ -3582,7 +3582,7 @@
         <v>44</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>199</v>
+        <v>295</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3614,7 +3614,7 @@
         <v>14</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3637,7 +3637,7 @@
         <v>12</v>
       </c>
       <c r="G77" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H77" t="s">
         <v>169</v>
@@ -3646,7 +3646,7 @@
         <v>14</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3669,7 +3669,7 @@
         <v>12</v>
       </c>
       <c r="G78" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H78" t="s">
         <v>170</v>
@@ -3678,7 +3678,7 @@
         <v>14</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3701,7 +3701,7 @@
         <v>12</v>
       </c>
       <c r="G79" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H79" t="s">
         <v>170</v>
@@ -3710,7 +3710,7 @@
         <v>44</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3742,12 +3742,12 @@
         <v>12</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B81">
         <v>9</v>
@@ -3774,7 +3774,7 @@
         <v>14</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3806,7 +3806,7 @@
         <v>67</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>217</v>
+        <v>296</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3838,7 +3838,7 @@
         <v>38</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3875,7 +3875,7 @@
     </row>
     <row r="85" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B85">
         <v>21</v>
@@ -3902,7 +3902,7 @@
         <v>76</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3936,16 +3936,16 @@
         <v>12</v>
       </c>
       <c r="G87" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H87" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I87" t="s">
         <v>14</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3979,7 +3979,7 @@
         <v>44</v>
       </c>
       <c r="G89" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H89" t="s">
         <v>168</v>
@@ -3988,7 +3988,7 @@
         <v>76</v>
       </c>
       <c r="J89" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4004,7 +4004,7 @@
     </row>
     <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -4019,10 +4019,10 @@
         <v>49</v>
       </c>
       <c r="F91" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G91" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H91" t="s">
         <v>168</v>
@@ -4031,7 +4031,7 @@
         <v>14</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4054,7 +4054,7 @@
         <v>12</v>
       </c>
       <c r="G92" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H92" t="s">
         <v>175</v>
@@ -4063,7 +4063,7 @@
         <v>14</v>
       </c>
       <c r="J92" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4086,7 +4086,7 @@
         <v>50</v>
       </c>
       <c r="G93" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H93" t="s">
         <v>175</v>
@@ -4118,7 +4118,7 @@
         <v>50</v>
       </c>
       <c r="G94" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H94" t="s">
         <v>176</v>
@@ -4127,7 +4127,7 @@
         <v>14</v>
       </c>
       <c r="J94" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4150,7 +4150,7 @@
         <v>19</v>
       </c>
       <c r="G95" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H95" t="s">
         <v>173</v>
@@ -4159,7 +4159,7 @@
         <v>14</v>
       </c>
       <c r="J95" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -4230,7 +4230,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4692,7 +4692,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -4701,7 +4701,7 @@
         <v>146</v>
       </c>
       <c r="D37" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -5098,7 +5098,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B66">
         <v>9</v>
@@ -5308,7 +5308,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B81">
         <v>21</v>

</xml_diff>